<commit_message>
added alpha=1 to all xlsx
</commit_message>
<xml_diff>
--- a/outputs/fft-c__Clostridia.xlsx
+++ b/outputs/fft-c__Clostridia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanxinli/Desktop/project/BlindKameris-new/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238564BB-7AD5-0D44-BC62-0D94F6A2BF60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F860B7-DA90-2A46-A891-1AA73E517A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="28800" windowHeight="15880" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="g__Ruminococcus_E-LSVM" sheetId="1" r:id="rId1"/>
@@ -10714,7 +10714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -12119,7 +12121,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12203,12 +12205,12 @@
         <v>425</v>
       </c>
       <c r="B8" s="3">
-        <v>0.2121212121212121</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.78787878787878785</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>0.78</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>0.21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>